<commit_message>
Added Data Driven test
</commit_message>
<xml_diff>
--- a/src/test/java/trello/resources/testdata.xlsx
+++ b/src/test/java/trello/resources/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ameya/Projects/JPMCRestAssured/src/test/java/trello/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ameya/Projects/JPMCRestAssuredSep2021/src/test/java/trello/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C8A36F-DD33-034E-826E-634F5F8E2B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ED72D8-26B5-5A4A-8056-5E3D2321FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32380" yWindow="-1660" windowWidth="25440" windowHeight="15360" xr2:uid="{43A95DF9-77C4-6A4D-B0AA-05FAF99277B4}"/>
+    <workbookView xWindow="25600" yWindow="-3400" windowWidth="38400" windowHeight="21600" xr2:uid="{43A95DF9-77C4-6A4D-B0AA-05FAF99277B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Boardname</t>
   </si>
@@ -33,9 +33,6 @@
     <t>CardTitle</t>
   </si>
   <si>
-    <t>RABoard_2</t>
-  </si>
-  <si>
     <t>Learning Java</t>
   </si>
   <si>
@@ -54,13 +51,28 @@
     <t>Learning XYZ</t>
   </si>
   <si>
-    <t>ListName</t>
-  </si>
-  <si>
-    <t>To Do</t>
-  </si>
-  <si>
-    <t>Doing</t>
+    <t>CardDescription</t>
+  </si>
+  <si>
+    <t>Learning Java Description</t>
+  </si>
+  <si>
+    <t>Learning TestNG Description</t>
+  </si>
+  <si>
+    <t>Learning RestAssured Description</t>
+  </si>
+  <si>
+    <t>Learning Cucumber Description</t>
+  </si>
+  <si>
+    <t>Learning Mockito Description</t>
+  </si>
+  <si>
+    <t>Learning XYZ Description</t>
+  </si>
+  <si>
+    <t>Board_1453</t>
   </si>
 </sst>
 </file>
@@ -415,14 +427,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -430,76 +442,76 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Basic Authorization Code
</commit_message>
<xml_diff>
--- a/src/test/java/trello/resources/testdata.xlsx
+++ b/src/test/java/trello/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ameya/Projects/JPMCRestAssuredSep2021/src/test/java/trello/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ED72D8-26B5-5A4A-8056-5E3D2321FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BEA0A6-3A7B-A741-B562-6D18749941BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="-3400" windowWidth="38400" windowHeight="21600" xr2:uid="{43A95DF9-77C4-6A4D-B0AA-05FAF99277B4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Boardname</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Board_1453</t>
+  </si>
+  <si>
+    <t>Board_1452</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,7 +453,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>

</xml_diff>